<commit_message>
fixed issue where python script lost two subjects
</commit_message>
<xml_diff>
--- a/derivatives/df_TPJ.xlsx
+++ b/derivatives/df_TPJ.xlsx
@@ -19,16 +19,16 @@
     <t>sub</t>
   </si>
   <si>
-    <t>aTPJ_R-P_F-C</t>
+    <t>aTPJ_R_P_F_C</t>
   </si>
   <si>
-    <t>aTPJ_R-P_F-S</t>
+    <t>aTPJ_R_P_F_S</t>
   </si>
   <si>
-    <t>pTPJ_R-P_F-C</t>
+    <t>pTPJ_R_P_F_C</t>
   </si>
   <si>
-    <t>pTPJ_R-P_F-S</t>
+    <t>pTPJ_R_P_F_S</t>
   </si>
 </sst>
 </file>
@@ -386,7 +386,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:E44"/>
+  <dimension ref="A1:E46"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
@@ -819,325 +819,359 @@
     </row>
     <row r="26" spans="1:5">
       <c r="A26">
-        <v>3116</v>
+        <v>1303</v>
       </c>
       <c r="B26">
-        <v>-0.23925212793</v>
+        <v>0.0829808524</v>
       </c>
       <c r="C26">
-        <v>-0.04815396129999999</v>
+        <v>-0.02110848941999999</v>
       </c>
       <c r="D26">
-        <v>0.07760388448</v>
+        <v>-0.00618960030999996</v>
       </c>
       <c r="E26">
-        <v>0.03052608797000001</v>
+        <v>-0.16397736683</v>
       </c>
     </row>
     <row r="27" spans="1:5">
       <c r="A27">
-        <v>3122</v>
+        <v>3116</v>
       </c>
       <c r="B27">
-        <v>0.109689564443</v>
+        <v>-0.23925212793</v>
       </c>
       <c r="C27">
-        <v>-0.14174650074</v>
+        <v>-0.04815396129999999</v>
       </c>
       <c r="D27">
-        <v>0.03607110585000001</v>
+        <v>0.07760388448</v>
       </c>
       <c r="E27">
-        <v>-0.06322449183000001</v>
+        <v>0.03052608797000001</v>
       </c>
     </row>
     <row r="28" spans="1:5">
       <c r="A28">
-        <v>3125</v>
+        <v>3122</v>
       </c>
       <c r="B28">
-        <v>0.05503980562399999</v>
+        <v>0.109689564443</v>
       </c>
       <c r="C28">
-        <v>0.05351692240399999</v>
+        <v>-0.14174650074</v>
       </c>
       <c r="D28">
-        <v>0.04303667791</v>
+        <v>0.03607110585000001</v>
       </c>
       <c r="E28">
-        <v>0.01207597983</v>
+        <v>-0.06322449183000001</v>
       </c>
     </row>
     <row r="29" spans="1:5">
       <c r="A29">
-        <v>3140</v>
+        <v>3125</v>
       </c>
       <c r="B29">
-        <v>0.024945656147</v>
+        <v>0.05503980562399999</v>
       </c>
       <c r="C29">
-        <v>-0.05048287712</v>
+        <v>0.05351692240399999</v>
       </c>
       <c r="D29">
-        <v>-0.05284240237</v>
+        <v>0.04303667791</v>
       </c>
       <c r="E29">
-        <v>-0.21185441844</v>
+        <v>0.01207597983</v>
       </c>
     </row>
     <row r="30" spans="1:5">
       <c r="A30">
-        <v>3143</v>
+        <v>3140</v>
       </c>
       <c r="B30">
-        <v>0.4650902345</v>
+        <v>0.024945656147</v>
       </c>
       <c r="C30">
-        <v>0.48581754499</v>
+        <v>-0.05048287712</v>
       </c>
       <c r="D30">
-        <v>0.4744933755090001</v>
+        <v>-0.05284240237</v>
       </c>
       <c r="E30">
-        <v>0.6022480252600001</v>
+        <v>-0.21185441844</v>
       </c>
     </row>
     <row r="31" spans="1:5">
       <c r="A31">
-        <v>3152</v>
+        <v>3143</v>
       </c>
       <c r="B31">
-        <v>0.05086455533099998</v>
+        <v>0.4650902345</v>
       </c>
       <c r="C31">
-        <v>-0.1050420478</v>
+        <v>0.48581754499</v>
       </c>
       <c r="D31">
-        <v>0.16841803528</v>
+        <v>0.4744933755090001</v>
       </c>
       <c r="E31">
-        <v>0.06065092225</v>
+        <v>0.6022480252600001</v>
       </c>
     </row>
     <row r="32" spans="1:5">
       <c r="A32">
-        <v>3166</v>
+        <v>3152</v>
       </c>
       <c r="B32">
-        <v>0.24976355732</v>
+        <v>0.05086455533099998</v>
       </c>
       <c r="C32">
-        <v>0.15245342936</v>
+        <v>-0.1050420478</v>
       </c>
       <c r="D32">
-        <v>0.40723169232</v>
+        <v>0.16841803528</v>
       </c>
       <c r="E32">
-        <v>0.03794198596000001</v>
+        <v>0.06065092225</v>
       </c>
     </row>
     <row r="33" spans="1:5">
       <c r="A33">
-        <v>3167</v>
+        <v>3166</v>
       </c>
       <c r="B33">
-        <v>0.07748295347</v>
+        <v>0.24976355732</v>
       </c>
       <c r="C33">
-        <v>0.06677047483</v>
+        <v>0.15245342936</v>
       </c>
       <c r="D33">
-        <v>0.35918305491</v>
+        <v>0.40723169232</v>
       </c>
       <c r="E33">
-        <v>0.41602414027</v>
+        <v>0.03794198596000001</v>
       </c>
     </row>
     <row r="34" spans="1:5">
       <c r="A34">
-        <v>3170</v>
+        <v>3167</v>
       </c>
       <c r="B34">
-        <v>-0.19098126166</v>
+        <v>0.07748295347</v>
       </c>
       <c r="C34">
-        <v>0.05770407405000001</v>
+        <v>0.06677047483</v>
       </c>
       <c r="D34">
-        <v>0.17458624865</v>
+        <v>0.35918305491</v>
       </c>
       <c r="E34">
-        <v>0.08707896276999999</v>
+        <v>0.41602414027</v>
       </c>
     </row>
     <row r="35" spans="1:5">
       <c r="A35">
-        <v>3173</v>
+        <v>3170</v>
       </c>
       <c r="B35">
-        <v>0.17901112546</v>
+        <v>-0.19098126166</v>
       </c>
       <c r="C35">
-        <v>0.04623594425999999</v>
+        <v>0.05770407405000001</v>
       </c>
       <c r="D35">
-        <v>0.138281604254</v>
+        <v>0.17458624865</v>
       </c>
       <c r="E35">
-        <v>-0.029414658896</v>
+        <v>0.08707896276999999</v>
       </c>
     </row>
     <row r="36" spans="1:5">
       <c r="A36">
-        <v>3176</v>
+        <v>3173</v>
       </c>
       <c r="B36">
-        <v>0.06847420598999999</v>
+        <v>0.17901112546</v>
       </c>
       <c r="C36">
-        <v>0.01276505114</v>
+        <v>0.04623594425999999</v>
       </c>
       <c r="D36">
-        <v>-0.01235817266999999</v>
+        <v>0.138281604254</v>
       </c>
       <c r="E36">
-        <v>0.05253338749000001</v>
+        <v>-0.029414658896</v>
       </c>
     </row>
     <row r="37" spans="1:5">
       <c r="A37">
-        <v>3189</v>
+        <v>3176</v>
       </c>
       <c r="B37">
-        <v>-0.048733674896</v>
+        <v>0.06847420598999999</v>
       </c>
       <c r="C37">
-        <v>0.08989506823400001</v>
+        <v>0.01276505114</v>
       </c>
       <c r="D37">
-        <v>0.57289901046</v>
+        <v>-0.01235817266999999</v>
       </c>
       <c r="E37">
-        <v>0.371762889812</v>
+        <v>0.05253338749000001</v>
       </c>
     </row>
     <row r="38" spans="1:5">
       <c r="A38">
-        <v>3190</v>
+        <v>3189</v>
       </c>
       <c r="B38">
-        <v>0.16345618173</v>
+        <v>-0.048733674896</v>
       </c>
       <c r="C38">
-        <v>-0.09382702042</v>
+        <v>0.08989506823400001</v>
       </c>
       <c r="D38">
-        <v>0.01973975812000001</v>
+        <v>0.57289901046</v>
       </c>
       <c r="E38">
-        <v>-0.003729203009999987</v>
+        <v>0.371762889812</v>
       </c>
     </row>
     <row r="39" spans="1:5">
       <c r="A39">
-        <v>3199</v>
+        <v>3190</v>
       </c>
       <c r="B39">
-        <v>0.22549663369</v>
+        <v>0.16345618173</v>
       </c>
       <c r="C39">
-        <v>0.20531194771</v>
+        <v>-0.09382702042</v>
       </c>
       <c r="D39">
-        <v>0.177746595654</v>
+        <v>0.01973975812000001</v>
       </c>
       <c r="E39">
-        <v>0.22842368635</v>
+        <v>-0.003729203009999987</v>
       </c>
     </row>
     <row r="40" spans="1:5">
       <c r="A40">
-        <v>3200</v>
+        <v>3199</v>
       </c>
       <c r="B40">
-        <v>-0.23717310821</v>
+        <v>0.22549663369</v>
       </c>
       <c r="C40">
-        <v>-0.05773890540000003</v>
+        <v>0.20531194771</v>
       </c>
       <c r="D40">
-        <v>-0.3225002648899999</v>
+        <v>0.177746595654</v>
       </c>
       <c r="E40">
-        <v>0.05455065716000002</v>
+        <v>0.22842368635</v>
       </c>
     </row>
     <row r="41" spans="1:5">
       <c r="A41">
-        <v>3206</v>
+        <v>3200</v>
       </c>
       <c r="B41">
-        <v>0.04095031303699999</v>
+        <v>-0.23717310821</v>
       </c>
       <c r="C41">
-        <v>-0.001821437773000006</v>
+        <v>-0.05773890540000003</v>
       </c>
       <c r="D41">
-        <v>-0.10096501849</v>
+        <v>-0.3225002648899999</v>
       </c>
       <c r="E41">
-        <v>-0.04490134692</v>
+        <v>0.05455065716000002</v>
       </c>
     </row>
     <row r="42" spans="1:5">
       <c r="A42">
-        <v>3210</v>
+        <v>3206</v>
       </c>
       <c r="B42">
-        <v>0.055935082787</v>
+        <v>0.04095031303699999</v>
       </c>
       <c r="C42">
-        <v>-0.07890800592299999</v>
+        <v>-0.001821437773000006</v>
       </c>
       <c r="D42">
-        <v>0.43603451893</v>
+        <v>-0.10096501849</v>
       </c>
       <c r="E42">
-        <v>-0.10335988246</v>
+        <v>-0.04490134692</v>
       </c>
     </row>
     <row r="43" spans="1:5">
       <c r="A43">
-        <v>3212</v>
+        <v>3210</v>
       </c>
       <c r="B43">
-        <v>0.12417176385</v>
+        <v>0.055935082787</v>
       </c>
       <c r="C43">
-        <v>0.01857846904000001</v>
+        <v>-0.07890800592299999</v>
       </c>
       <c r="D43">
-        <v>-0.1896221339</v>
+        <v>0.43603451893</v>
       </c>
       <c r="E43">
-        <v>-0.18598617106</v>
+        <v>-0.10335988246</v>
       </c>
     </row>
     <row r="44" spans="1:5">
       <c r="A44">
+        <v>3212</v>
+      </c>
+      <c r="B44">
+        <v>0.12417176385</v>
+      </c>
+      <c r="C44">
+        <v>0.01857846904000001</v>
+      </c>
+      <c r="D44">
+        <v>-0.1896221339</v>
+      </c>
+      <c r="E44">
+        <v>-0.18598617106</v>
+      </c>
+    </row>
+    <row r="45" spans="1:5">
+      <c r="A45">
         <v>3218</v>
       </c>
-      <c r="B44">
+      <c r="B45">
         <v>0.09012457586999999</v>
       </c>
-      <c r="C44">
+      <c r="C45">
         <v>0.203674259068</v>
       </c>
-      <c r="D44">
+      <c r="D45">
         <v>-0.14879623426</v>
       </c>
-      <c r="E44">
+      <c r="E45">
         <v>0.04727141383000003</v>
+      </c>
+    </row>
+    <row r="46" spans="1:5">
+      <c r="A46">
+        <v>3220</v>
+      </c>
+      <c r="B46">
+        <v>0.07862091610000001</v>
+      </c>
+      <c r="C46">
+        <v>-0.08206761560000002</v>
+      </c>
+      <c r="D46">
+        <v>0.3183748924300001</v>
+      </c>
+      <c r="E46">
+        <v>-0.04529498433000001</v>
       </c>
     </row>
   </sheetData>

</xml_diff>